<commit_message>
NodoTracker lee JSON formulario
</commit_message>
<xml_diff>
--- a/Pruebas/New Microsoft Excel Worksheet.xlsx
+++ b/Pruebas/New Microsoft Excel Worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Desktop\Facultad\4to\2doCuatrimestre\SistemasDistribuidos\tp-sistemas-distribuidos\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ADB38A-A013-4BD4-B9A4-B713E0A98153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F221A7C-857B-4478-A530-4C5C9BD09C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3195" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Nodo 1</t>
   </si>
@@ -97,14 +97,40 @@
   </si>
   <si>
     <t>sig</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>CANT NODOS</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>IP SIGUIENTE</t>
+  </si>
+  <si>
+    <t>PORT SIGUIENTE</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,11 +158,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D11"/>
+      <selection activeCell="I14" activeCellId="1" sqref="B5 I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +512,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
@@ -540,11 +567,41 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>27015</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D7:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nodoTracker con funciones store, cliente.js y servidor.js como protitipos
</commit_message>
<xml_diff>
--- a/Pruebas/New Microsoft Excel Worksheet.xlsx
+++ b/Pruebas/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Desktop\Facultad\4to\2doCuatrimestre\SistemasDistribuidos\tp-sistemas-distribuidos\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F221A7C-857B-4478-A530-4C5C9BD09C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D25BE61-375E-41B2-A94F-AD743067FCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Nodo 1</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>HASH 3</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" activeCellId="1" sqref="B5 I14"/>
+      <selection activeCell="I10" sqref="I10:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,101 +509,119 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="G7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
+      <c r="G8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="C16">
+      <c r="C22">
         <v>27015</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D7:D11"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>